<commit_message>
Rectification (word + Excel RebuiLT)
</commit_message>
<xml_diff>
--- a/2 - Bilans/2022-2023/Unipoly_Bilan_Quadrimestriel_22-23.xlsx
+++ b/2 - Bilans/2022-2023/Unipoly_Bilan_Quadrimestriel_22-23.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/theodoresavary/Desktop/Unipoly/UPSecretrariat/2 - Bilans/2022-2023/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47B50417-854D-B843-B763-492E45F2E29D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01BB41D9-DE8C-2045-A0FB-A64A8FCDAAE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="779" xr2:uid="{34F8AD7C-3B1E-42A7-8AF2-50C33241ADA4}"/>
   </bookViews>
@@ -1122,9 +1122,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75A55C92-786C-4AB3-96FC-7473E4CC0A9B}">
   <dimension ref="A1:Y70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="M19" sqref="M19:M20"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="3" topLeftCell="J1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="M57" sqref="M57:M58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="16" zeroHeight="1"/>
@@ -2667,11 +2667,11 @@
       </c>
       <c r="L31" s="8">
         <f>L33+L35+L37+L39+L41+L43+L45+L47+L49+L51+L53+L55+L57+L59+L61+L63+L65</f>
-        <v>0</v>
+        <v>4352.4800000000005</v>
       </c>
       <c r="M31" s="33">
         <f>L31-L32+K31</f>
-        <v>-2211.6800000000003</v>
+        <v>-10000.959999999999</v>
       </c>
       <c r="N31" s="8">
         <f>N33+N35+N37+N39+N41+N43+N45+N47+N49+N51+N53+N55+N57+N59+N61+N63+N65</f>
@@ -2679,7 +2679,7 @@
       </c>
       <c r="O31" s="33">
         <f>N31-N32+M31</f>
-        <v>-2211.6800000000003</v>
+        <v>-10000.959999999999</v>
       </c>
       <c r="P31" s="6">
         <f>P33+P35+P37+P39+P41+P43+P45+P47+P49+P51+P53+P55+P57+P59+P61+P63+P65</f>
@@ -2687,7 +2687,7 @@
       </c>
       <c r="Q31" s="34">
         <f>P31-P32+O31</f>
-        <v>-6618.02</v>
+        <v>-14407.3</v>
       </c>
       <c r="R31" s="6">
         <f>R33+R35+R37+R39+R41+R43+R45+R47+R49+R51+R53+R55+R57+R59+R61+R63+R65</f>
@@ -2695,7 +2695,7 @@
       </c>
       <c r="S31" s="34">
         <f>R31-R32+Q31</f>
-        <v>-34898.020000000004</v>
+        <v>-42687.3</v>
       </c>
       <c r="T31" s="8">
         <f>T33+T35+T37+T39+T41+T43+T45+T47+T49+T51+T53+T55+T57+T59+T61+T63+T65</f>
@@ -2703,7 +2703,7 @@
       </c>
       <c r="U31" s="33">
         <f>T31-T32+S31</f>
-        <v>-29085.700000000004</v>
+        <v>-36874.980000000003</v>
       </c>
     </row>
     <row r="32" spans="2:21">
@@ -2731,7 +2731,7 @@
       <c r="K32" s="34"/>
       <c r="L32" s="7">
         <f>L34+L36+L38+L40+L42+L44+L46+L48+L50+L52+L54+L56+L58+L60+L62+L64+L66</f>
-        <v>0</v>
+        <v>12141.76</v>
       </c>
       <c r="M32" s="34"/>
       <c r="N32" s="7">
@@ -2791,11 +2791,11 @@
       </c>
       <c r="L33" s="6">
         <f>API_Clôtures!$C$3</f>
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="M33" s="34">
         <f t="shared" ref="M33" si="39">L33-L34+K33</f>
-        <v>-998.79</v>
+        <v>-938.79</v>
       </c>
       <c r="N33" s="6">
         <f>API_Clôtures!$D$3</f>
@@ -2803,24 +2803,24 @@
       </c>
       <c r="O33" s="34">
         <f t="shared" ref="O33" si="40">N33-N34+M33</f>
-        <v>-998.79</v>
+        <v>-938.79</v>
       </c>
       <c r="P33" s="6"/>
       <c r="Q33" s="34">
         <f>P33-P34+O33</f>
-        <v>-998.79</v>
+        <v>-938.79</v>
       </c>
       <c r="R33" s="6"/>
       <c r="S33" s="34">
         <f t="shared" ref="S33" si="41">R33-R34+Q33</f>
-        <v>-1148.79</v>
+        <v>-1088.79</v>
       </c>
       <c r="T33" s="6">
         <v>917.79</v>
       </c>
       <c r="U33" s="34">
         <f t="shared" ref="U33" si="42">T33-T34+S33</f>
-        <v>-231</v>
+        <v>-171</v>
       </c>
     </row>
     <row r="34" spans="2:21">
@@ -3019,7 +3019,7 @@
       </c>
       <c r="M37" s="34">
         <f t="shared" ref="M37" si="53">L37-L38+K37</f>
-        <v>4777.0999999999995</v>
+        <v>4702.4399999999996</v>
       </c>
       <c r="N37" s="6">
         <f>CASTOR_Clôtures!$D$3</f>
@@ -3027,24 +3027,24 @@
       </c>
       <c r="O37" s="34">
         <f t="shared" ref="O37" si="54">N37-N38+M37</f>
-        <v>4777.0999999999995</v>
+        <v>4702.4399999999996</v>
       </c>
       <c r="P37" s="6"/>
       <c r="Q37" s="34">
         <f>P37-P38+O37</f>
-        <v>370.75999999999931</v>
+        <v>296.09999999999945</v>
       </c>
       <c r="R37" s="6"/>
       <c r="S37" s="34">
         <f t="shared" ref="S37" si="55">R37-R38+Q37</f>
-        <v>-1229.2400000000007</v>
+        <v>-1303.9000000000005</v>
       </c>
       <c r="T37" s="6">
         <v>1445.73</v>
       </c>
       <c r="U37" s="55">
         <f t="shared" ref="U37" si="56">T37-T38+S37</f>
-        <v>-2162.8000000000006</v>
+        <v>-2237.4600000000005</v>
       </c>
     </row>
     <row r="38" spans="2:21">
@@ -3069,7 +3069,7 @@
       <c r="K38" s="34"/>
       <c r="L38" s="7">
         <f>CASTOR_Clôtures!$C$5</f>
-        <v>0</v>
+        <v>74.66</v>
       </c>
       <c r="M38" s="34"/>
       <c r="N38" s="7">
@@ -3132,7 +3132,7 @@
       </c>
       <c r="M39" s="34">
         <f t="shared" ref="M39" si="60">L39-L40+K39</f>
-        <v>-485.03</v>
+        <v>-500.53</v>
       </c>
       <c r="N39" s="6">
         <f>DEBOUC_Clôtures!$D$3</f>
@@ -3140,24 +3140,24 @@
       </c>
       <c r="O39" s="34">
         <f t="shared" ref="O39" si="61">N39-N40+M39</f>
-        <v>-485.03</v>
+        <v>-500.53</v>
       </c>
       <c r="P39" s="6"/>
       <c r="Q39" s="34">
         <f>P39-P40+O39</f>
-        <v>-485.03</v>
+        <v>-500.53</v>
       </c>
       <c r="R39" s="6"/>
       <c r="S39" s="34">
         <f t="shared" ref="S39" si="62">R39-R40+Q39</f>
-        <v>-485.03</v>
+        <v>-500.53</v>
       </c>
       <c r="T39" s="6">
         <v>128.69999999999999</v>
       </c>
       <c r="U39" s="34">
         <f t="shared" ref="U39" si="63">T39-T40+S39</f>
-        <v>-356.33</v>
+        <v>-371.83</v>
       </c>
     </row>
     <row r="40" spans="2:21">
@@ -3182,7 +3182,7 @@
       <c r="K40" s="34"/>
       <c r="L40" s="7">
         <f>DEBOUC_Clôtures!$C$5</f>
-        <v>0</v>
+        <v>15.5</v>
       </c>
       <c r="M40" s="34"/>
       <c r="N40" s="7">
@@ -3241,7 +3241,7 @@
       </c>
       <c r="M41" s="34">
         <f t="shared" ref="M41" si="66">L41-L42+K41</f>
-        <v>-1236</v>
+        <v>-1764.35</v>
       </c>
       <c r="N41" s="6">
         <f>EVA_Clôtures!$D$3</f>
@@ -3249,24 +3249,24 @@
       </c>
       <c r="O41" s="34">
         <f t="shared" ref="O41" si="67">N41-N42+M41</f>
-        <v>-1236</v>
+        <v>-1764.35</v>
       </c>
       <c r="P41" s="6"/>
       <c r="Q41" s="34">
         <f>P41-P42+O41</f>
-        <v>-1236</v>
+        <v>-1764.35</v>
       </c>
       <c r="R41" s="6"/>
       <c r="S41" s="34">
         <f t="shared" ref="S41" si="68">R41-R42+Q41</f>
-        <v>-1836</v>
+        <v>-2364.35</v>
       </c>
       <c r="T41" s="6">
         <v>81.900000000000006</v>
       </c>
       <c r="U41" s="34">
         <f t="shared" ref="U41" si="69">T41-T42+S41</f>
-        <v>-1869.05</v>
+        <v>-2397.4</v>
       </c>
     </row>
     <row r="42" spans="2:21">
@@ -3289,7 +3289,7 @@
       <c r="K42" s="34"/>
       <c r="L42" s="7">
         <f>EVA_Clôtures!$C$5</f>
-        <v>0</v>
+        <v>528.35</v>
       </c>
       <c r="M42" s="34"/>
       <c r="N42" s="7">
@@ -3764,7 +3764,7 @@
       </c>
       <c r="M51" s="34">
         <f t="shared" ref="M51" si="98">L51-L52+K51</f>
-        <v>-1100</v>
+        <v>-1205.95</v>
       </c>
       <c r="N51" s="6">
         <f>JARDIN_Clôtures!$D$3</f>
@@ -3772,24 +3772,24 @@
       </c>
       <c r="O51" s="34">
         <f t="shared" ref="O51" si="99">N51-N52+M51</f>
-        <v>-1100</v>
+        <v>-1205.95</v>
       </c>
       <c r="P51" s="6"/>
       <c r="Q51" s="34">
         <f>P51-P52+O51</f>
-        <v>-1100</v>
+        <v>-1205.95</v>
       </c>
       <c r="R51" s="6"/>
       <c r="S51" s="34">
         <f t="shared" ref="S51" si="100">R51-R52+Q51</f>
-        <v>-1100</v>
+        <v>-1205.95</v>
       </c>
       <c r="T51" s="6">
         <v>1022.8</v>
       </c>
       <c r="U51" s="34">
         <f t="shared" ref="U51" si="101">T51-T52+S51</f>
-        <v>-289.20000000000005</v>
+        <v>-395.15000000000009</v>
       </c>
     </row>
     <row r="52" spans="2:21">
@@ -3810,7 +3810,7 @@
       <c r="K52" s="34"/>
       <c r="L52" s="7">
         <f>JARDIN_Clôtures!$C$5</f>
-        <v>0</v>
+        <v>105.95</v>
       </c>
       <c r="M52" s="34"/>
       <c r="N52" s="7">
@@ -3868,31 +3868,31 @@
       </c>
       <c r="M53" s="34">
         <f t="shared" ref="M53" si="105">L53-L54+K53</f>
-        <v>1116.4299999999998</v>
+        <v>629.18999999999983</v>
       </c>
       <c r="N53" s="6">
         <v>0</v>
       </c>
       <c r="O53" s="34">
         <f t="shared" ref="O53" si="106">N53-N54+M53</f>
-        <v>1116.4299999999998</v>
+        <v>629.18999999999983</v>
       </c>
       <c r="P53" s="6"/>
       <c r="Q53" s="34">
         <f>P53-P54+O53</f>
-        <v>1116.4299999999998</v>
+        <v>629.18999999999983</v>
       </c>
       <c r="R53" s="6"/>
       <c r="S53" s="34">
         <f t="shared" ref="S53" si="107">R53-R54+Q53</f>
-        <v>1116.4299999999998</v>
+        <v>629.18999999999983</v>
       </c>
       <c r="T53" s="6">
         <v>1456.25</v>
       </c>
       <c r="U53" s="34">
         <f t="shared" ref="U53" si="108">T53-T54+S53</f>
-        <v>2572.6799999999998</v>
+        <v>2085.4399999999996</v>
       </c>
     </row>
     <row r="54" spans="2:21">
@@ -3913,7 +3913,7 @@
       <c r="K54" s="34"/>
       <c r="L54" s="7">
         <f>MEUBLE_Clôtures!$C$5</f>
-        <v>0</v>
+        <v>487.24</v>
       </c>
       <c r="M54" s="34"/>
       <c r="N54" s="7">
@@ -3964,11 +3964,11 @@
       </c>
       <c r="L55" s="6">
         <f>MEUBLE_Clôtures!$C$2</f>
-        <v>0</v>
+        <v>370.2</v>
       </c>
       <c r="M55" s="34">
         <f t="shared" ref="M55" si="111">L55-L56+K55</f>
-        <v>1478.71</v>
+        <v>1683.91</v>
       </c>
       <c r="N55" s="6">
         <f>MEUBLE_Clôtures!$D$2</f>
@@ -3976,24 +3976,24 @@
       </c>
       <c r="O55" s="34">
         <f t="shared" ref="O55" si="112">N55-N56+M55</f>
-        <v>1478.71</v>
+        <v>1683.91</v>
       </c>
       <c r="P55" s="6"/>
       <c r="Q55" s="34">
         <f>P55-P56+O55</f>
-        <v>1478.71</v>
+        <v>1683.91</v>
       </c>
       <c r="R55" s="6"/>
       <c r="S55" s="34">
         <f t="shared" ref="S55" si="113">R55-R56+Q55</f>
-        <v>-151.28999999999996</v>
+        <v>53.910000000000082</v>
       </c>
       <c r="T55" s="6">
         <v>1545</v>
       </c>
       <c r="U55" s="34">
         <f t="shared" ref="U55" si="114">T55-T56+S55</f>
-        <v>764.51</v>
+        <v>969.71</v>
       </c>
     </row>
     <row r="56" spans="2:21">
@@ -4014,7 +4014,7 @@
       <c r="K56" s="34"/>
       <c r="L56" s="7">
         <f>MEUBLE_Clôtures!$C$6</f>
-        <v>0</v>
+        <v>165</v>
       </c>
       <c r="M56" s="34"/>
       <c r="N56" s="7">
@@ -4068,11 +4068,11 @@
       </c>
       <c r="L57" s="6">
         <f>DUDU_Clôtures!$C$3</f>
-        <v>0</v>
+        <v>3916.98</v>
       </c>
       <c r="M57" s="34">
         <f t="shared" ref="M57" si="118">L57-L58+K57</f>
-        <v>0</v>
+        <v>-3171.68</v>
       </c>
       <c r="N57" s="6">
         <f>DUDU_Clôtures!$D$3</f>
@@ -4080,24 +4080,24 @@
       </c>
       <c r="O57" s="34">
         <f t="shared" ref="O57" si="119">N57-N58+M57</f>
-        <v>0</v>
+        <v>-3171.68</v>
       </c>
       <c r="P57" s="6"/>
       <c r="Q57" s="34">
         <f>P57-P58+O57</f>
-        <v>0</v>
+        <v>-3171.68</v>
       </c>
       <c r="R57" s="6"/>
       <c r="S57" s="34">
         <f t="shared" ref="S57" si="120">R57-R58+Q57</f>
-        <v>-10000</v>
+        <v>-13171.68</v>
       </c>
       <c r="T57" s="6">
         <v>6506.55</v>
       </c>
       <c r="U57" s="34">
         <f t="shared" ref="U57" si="121">T57-T58+S57</f>
-        <v>-10000</v>
+        <v>-13171.68</v>
       </c>
     </row>
     <row r="58" spans="2:21">
@@ -4118,7 +4118,7 @@
       <c r="K58" s="34"/>
       <c r="L58" s="7">
         <f>DUDU_Clôtures!$C$5</f>
-        <v>0</v>
+        <v>7088.66</v>
       </c>
       <c r="M58" s="34"/>
       <c r="N58" s="7">
@@ -4176,31 +4176,31 @@
       </c>
       <c r="M59" s="34">
         <f t="shared" ref="M59" si="124">L59-L60+K59</f>
-        <v>-6183.22</v>
+        <v>-7927.4500000000007</v>
       </c>
       <c r="N59" s="6">
         <v>0</v>
       </c>
       <c r="O59" s="34">
         <f t="shared" ref="O59" si="125">N59-N60+M59</f>
-        <v>-6183.22</v>
+        <v>-7927.4500000000007</v>
       </c>
       <c r="P59" s="6"/>
       <c r="Q59" s="34">
         <f>P59-P60+O59</f>
-        <v>-6183.22</v>
+        <v>-7927.4500000000007</v>
       </c>
       <c r="R59" s="6"/>
       <c r="S59" s="34">
         <f>R59-R60+Q59</f>
-        <v>-6683.22</v>
+        <v>-8427.4500000000007</v>
       </c>
       <c r="T59" s="6">
         <v>1576.53</v>
       </c>
       <c r="U59" s="34">
         <f t="shared" ref="U59" si="126">T59-T60+S59</f>
-        <v>-5106.6900000000005</v>
+        <v>-6850.920000000001</v>
       </c>
     </row>
     <row r="60" spans="2:21" ht="15.5" customHeight="1">
@@ -4221,7 +4221,7 @@
       <c r="K60" s="34"/>
       <c r="L60" s="7">
         <f>UPFL_Clôtures!$C$5</f>
-        <v>0</v>
+        <v>1744.23</v>
       </c>
       <c r="M60" s="34"/>
       <c r="N60" s="7">
@@ -4374,11 +4374,11 @@
       </c>
       <c r="L63" s="6">
         <f>FNR_Clôtures!$C$2</f>
-        <v>0</v>
+        <v>5.3</v>
       </c>
       <c r="M63" s="34">
         <f>L63-L64+K63</f>
-        <v>-2103.16</v>
+        <v>-4030.0299999999997</v>
       </c>
       <c r="N63" s="6">
         <f>FNR_Clôtures!$D$2</f>
@@ -4386,24 +4386,24 @@
       </c>
       <c r="O63" s="34">
         <f>N63-N64+M63</f>
-        <v>-2103.16</v>
+        <v>-4030.0299999999997</v>
       </c>
       <c r="P63" s="6"/>
       <c r="Q63" s="34">
         <f>P63-P64+O63</f>
-        <v>-2103.16</v>
+        <v>-4030.0299999999997</v>
       </c>
       <c r="R63" s="6"/>
       <c r="S63" s="34">
         <f t="shared" ref="S63" si="127">R63-R64+Q63</f>
-        <v>-2103.16</v>
+        <v>-4030.0299999999997</v>
       </c>
       <c r="T63" s="6">
         <v>720.75</v>
       </c>
       <c r="U63" s="34">
         <f>T63-T64+S63</f>
-        <v>-1457.0099999999998</v>
+        <v>-3383.8799999999997</v>
       </c>
     </row>
     <row r="64" spans="2:21">
@@ -4423,7 +4423,7 @@
       <c r="K64" s="34"/>
       <c r="L64" s="7">
         <f>FNR_Clôtures!$C$4</f>
-        <v>0</v>
+        <v>1932.17</v>
       </c>
       <c r="M64" s="34"/>
       <c r="N64" s="7">
@@ -4576,27 +4576,27 @@
       <c r="K67" s="35"/>
       <c r="L67" s="35">
         <f>M5+M7+M31</f>
-        <v>-17240.55</v>
+        <v>-25029.829999999998</v>
       </c>
       <c r="M67" s="35"/>
       <c r="N67" s="35">
         <f>O5+O7+O31</f>
-        <v>-17240.55</v>
+        <v>-25029.829999999998</v>
       </c>
       <c r="O67" s="35"/>
       <c r="P67" s="35">
         <f>Q5+Q7+Q31</f>
-        <v>-17240.55</v>
+        <v>-25029.829999999998</v>
       </c>
       <c r="Q67" s="35"/>
       <c r="R67" s="35">
         <f>S5+S7+S31</f>
-        <v>-17240.550000000003</v>
+        <v>-25029.83</v>
       </c>
       <c r="S67" s="35"/>
       <c r="T67" s="35">
         <f>U5+U7+U31</f>
-        <v>-16594.400000000005</v>
+        <v>-24383.680000000004</v>
       </c>
       <c r="U67" s="35"/>
     </row>
@@ -5094,7 +5094,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E5"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -5383,7 +5383,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -5416,14 +5416,14 @@
         <v>119</v>
       </c>
       <c r="C2" s="18">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="D2" s="18">
         <v>0</v>
       </c>
       <c r="E2" s="20">
         <f>SUM(B2:D2)</f>
-        <v>119</v>
+        <v>179</v>
       </c>
       <c r="F2" s="22"/>
       <c r="G2" s="22"/>
@@ -5438,7 +5438,7 @@
       </c>
       <c r="C3" s="19">
         <f>SUM(C2:C2)</f>
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="D3" s="19">
         <f>SUM(D2:D2)</f>
@@ -5446,7 +5446,7 @@
       </c>
       <c r="E3" s="19">
         <f>SUM(E2:E2)</f>
-        <v>119</v>
+        <v>179</v>
       </c>
       <c r="F3" s="22"/>
       <c r="G3" s="22"/>
@@ -5757,7 +5757,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -5833,14 +5833,14 @@
         <v>789.99</v>
       </c>
       <c r="C4" s="18">
-        <v>0</v>
+        <v>74.66</v>
       </c>
       <c r="D4" s="18">
         <v>0</v>
       </c>
       <c r="E4" s="20">
         <f>SUM(B4:D4)</f>
-        <v>789.99</v>
+        <v>864.65</v>
       </c>
       <c r="F4" s="22"/>
       <c r="G4" s="22"/>
@@ -5855,7 +5855,7 @@
       </c>
       <c r="C5" s="21">
         <f>SUM(C4:C4)</f>
-        <v>0</v>
+        <v>74.66</v>
       </c>
       <c r="D5" s="21">
         <f>SUM(D4:D4)</f>
@@ -5863,7 +5863,7 @@
       </c>
       <c r="E5" s="21">
         <f>SUM(E4:E4)</f>
-        <v>789.99</v>
+        <v>864.65</v>
       </c>
       <c r="F5" s="22"/>
       <c r="G5" s="22"/>
@@ -5935,7 +5935,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -6011,14 +6011,14 @@
         <v>26.33</v>
       </c>
       <c r="C4" s="18">
-        <v>0</v>
+        <v>15.5</v>
       </c>
       <c r="D4" s="18">
         <v>0</v>
       </c>
       <c r="E4" s="20">
         <f>SUM(B4:D4)</f>
-        <v>26.33</v>
+        <v>41.83</v>
       </c>
       <c r="F4" s="22"/>
       <c r="G4" s="22"/>
@@ -6033,7 +6033,7 @@
       </c>
       <c r="C5" s="21">
         <f>SUM(C4:C4)</f>
-        <v>0</v>
+        <v>15.5</v>
       </c>
       <c r="D5" s="21">
         <f>SUM(D4:D4)</f>
@@ -6041,7 +6041,7 @@
       </c>
       <c r="E5" s="21">
         <f>SUM(E4:E4)</f>
-        <v>26.33</v>
+        <v>41.83</v>
       </c>
       <c r="F5" s="22"/>
       <c r="G5" s="22"/>
@@ -6113,7 +6113,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -6189,14 +6189,14 @@
         <v>269.05</v>
       </c>
       <c r="C4" s="18">
-        <v>0</v>
+        <v>528.35</v>
       </c>
       <c r="D4" s="18">
         <v>0</v>
       </c>
       <c r="E4" s="20">
         <f>SUM(B4:D4)</f>
-        <v>269.05</v>
+        <v>797.40000000000009</v>
       </c>
       <c r="F4" s="22"/>
       <c r="G4" s="22"/>
@@ -6211,7 +6211,7 @@
       </c>
       <c r="C5" s="21">
         <f>SUM(C4:C4)</f>
-        <v>0</v>
+        <v>528.35</v>
       </c>
       <c r="D5" s="21">
         <f>SUM(D4:D4)</f>
@@ -6219,7 +6219,7 @@
       </c>
       <c r="E5" s="21">
         <f>SUM(E4:E4)</f>
-        <v>269.05</v>
+        <v>797.40000000000009</v>
       </c>
       <c r="F5" s="22"/>
       <c r="G5" s="22"/>
@@ -6911,7 +6911,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -6987,14 +6987,14 @@
         <v>50</v>
       </c>
       <c r="C4" s="18">
-        <v>0</v>
+        <v>105.95</v>
       </c>
       <c r="D4" s="18">
         <v>0</v>
       </c>
       <c r="E4" s="20">
         <f>SUM(B4:D4)</f>
-        <v>50</v>
+        <v>155.94999999999999</v>
       </c>
       <c r="F4" s="22"/>
       <c r="G4" s="22"/>
@@ -7009,7 +7009,7 @@
       </c>
       <c r="C5" s="21">
         <f>SUM(C4:C4)</f>
-        <v>0</v>
+        <v>105.95</v>
       </c>
       <c r="D5" s="21">
         <f>SUM(D4:D4)</f>
@@ -7017,7 +7017,7 @@
       </c>
       <c r="E5" s="21">
         <f>SUM(E4:E4)</f>
-        <v>50</v>
+        <v>155.94999999999999</v>
       </c>
       <c r="F5" s="22"/>
       <c r="G5" s="22"/>
@@ -7267,7 +7267,7 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -7300,14 +7300,14 @@
         <v>2061.25</v>
       </c>
       <c r="C2" s="18">
-        <v>0</v>
+        <v>370.2</v>
       </c>
       <c r="D2" s="18">
         <v>0</v>
       </c>
       <c r="E2" s="20">
         <f>SUM(B2:D2)</f>
-        <v>2061.25</v>
+        <v>2431.4499999999998</v>
       </c>
       <c r="F2" s="22"/>
       <c r="G2" s="22"/>
@@ -7320,14 +7320,14 @@
         <v>1788.71</v>
       </c>
       <c r="C3" s="18">
-        <v>0</v>
+        <v>530.79</v>
       </c>
       <c r="D3" s="18">
         <v>0</v>
       </c>
       <c r="E3" s="20">
         <f>SUM(B3:D3)</f>
-        <v>1788.71</v>
+        <v>2319.5</v>
       </c>
       <c r="F3" s="22"/>
       <c r="G3" s="22"/>
@@ -7342,7 +7342,7 @@
       </c>
       <c r="C4" s="19">
         <f>SUM(C2:C3)</f>
-        <v>0</v>
+        <v>900.99</v>
       </c>
       <c r="D4" s="19">
         <f>SUM(D2:D3)</f>
@@ -7350,7 +7350,7 @@
       </c>
       <c r="E4" s="19">
         <f>SUM(E2:E2)</f>
-        <v>2061.25</v>
+        <v>2431.4499999999998</v>
       </c>
       <c r="F4" s="22"/>
       <c r="G4" s="22"/>
@@ -7363,14 +7363,14 @@
         <v>764.82</v>
       </c>
       <c r="C5" s="18">
-        <v>0</v>
+        <v>487.24</v>
       </c>
       <c r="D5" s="18">
         <v>0</v>
       </c>
       <c r="E5" s="20">
         <f>SUM(B5:D5)</f>
-        <v>764.82</v>
+        <v>1252.06</v>
       </c>
       <c r="F5" s="22"/>
       <c r="G5" s="22"/>
@@ -7383,14 +7383,14 @@
         <v>0</v>
       </c>
       <c r="C6" s="18">
-        <v>0</v>
+        <v>165</v>
       </c>
       <c r="D6" s="18">
         <v>0</v>
       </c>
       <c r="E6" s="20">
         <f>SUM(B6:D6)</f>
-        <v>0</v>
+        <v>165</v>
       </c>
       <c r="F6" s="22"/>
       <c r="G6" s="22"/>
@@ -7405,7 +7405,7 @@
       </c>
       <c r="C7" s="21">
         <f>SUM(C5:C5)</f>
-        <v>0</v>
+        <v>487.24</v>
       </c>
       <c r="D7" s="21">
         <f>SUM(D5:D5)</f>
@@ -7413,7 +7413,7 @@
       </c>
       <c r="E7" s="21">
         <f>SUM(E5:E6)</f>
-        <v>764.82</v>
+        <v>1417.06</v>
       </c>
       <c r="F7" s="22"/>
       <c r="G7" s="22"/>
@@ -7485,7 +7485,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -7518,14 +7518,14 @@
         <v>0</v>
       </c>
       <c r="C2" s="18">
-        <v>0</v>
+        <v>3916.98</v>
       </c>
       <c r="D2" s="18">
         <v>0</v>
       </c>
       <c r="E2" s="20">
         <f>SUM(B2:D2)</f>
-        <v>0</v>
+        <v>3916.98</v>
       </c>
       <c r="F2" s="22"/>
       <c r="G2" s="22"/>
@@ -7540,7 +7540,7 @@
       </c>
       <c r="C3" s="19">
         <f>SUM(C2:C2)</f>
-        <v>0</v>
+        <v>3916.98</v>
       </c>
       <c r="D3" s="19">
         <f>SUM(D2:D2)</f>
@@ -7548,7 +7548,7 @@
       </c>
       <c r="E3" s="19">
         <f>SUM(E2:E2)</f>
-        <v>0</v>
+        <v>3916.98</v>
       </c>
       <c r="F3" s="22"/>
       <c r="G3" s="22"/>
@@ -7561,14 +7561,14 @@
         <v>0</v>
       </c>
       <c r="C4" s="18">
-        <v>0</v>
+        <v>7088.66</v>
       </c>
       <c r="D4" s="18">
         <v>0</v>
       </c>
       <c r="E4" s="20">
         <f>SUM(B4:D4)</f>
-        <v>0</v>
+        <v>7088.66</v>
       </c>
       <c r="F4" s="22"/>
       <c r="G4" s="22"/>
@@ -7583,7 +7583,7 @@
       </c>
       <c r="C5" s="21">
         <f>SUM(C4:C4)</f>
-        <v>0</v>
+        <v>7088.66</v>
       </c>
       <c r="D5" s="21">
         <f>SUM(D4:D4)</f>
@@ -7591,7 +7591,7 @@
       </c>
       <c r="E5" s="21">
         <f>SUM(E4:E4)</f>
-        <v>0</v>
+        <v>7088.66</v>
       </c>
       <c r="F5" s="22"/>
       <c r="G5" s="22"/>
@@ -7663,7 +7663,7 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -7716,14 +7716,14 @@
         <v>2498</v>
       </c>
       <c r="C3" s="18">
-        <v>0</v>
+        <v>2363.5</v>
       </c>
       <c r="D3" s="18">
         <v>0</v>
       </c>
       <c r="E3" s="20">
         <f>SUM(B3:D3)</f>
-        <v>2498</v>
+        <v>4861.5</v>
       </c>
       <c r="F3" s="22"/>
       <c r="G3" s="22"/>
@@ -7738,7 +7738,7 @@
       </c>
       <c r="C4" s="19">
         <f>SUM(C2:C3)</f>
-        <v>0</v>
+        <v>2363.5</v>
       </c>
       <c r="D4" s="19">
         <f>SUM(D2:D3)</f>
@@ -7746,7 +7746,7 @@
       </c>
       <c r="E4" s="19">
         <f>SUM(E2:E3)</f>
-        <v>4224.53</v>
+        <v>6588.03</v>
       </c>
       <c r="F4" s="22"/>
       <c r="G4" s="22"/>
@@ -7759,14 +7759,14 @@
         <v>1379.75</v>
       </c>
       <c r="C5" s="18">
-        <v>0</v>
+        <v>1744.23</v>
       </c>
       <c r="D5" s="18">
         <v>0</v>
       </c>
       <c r="E5" s="20">
         <f>SUM(B5:D5)</f>
-        <v>1379.75</v>
+        <v>3123.98</v>
       </c>
       <c r="F5" s="22"/>
       <c r="G5" s="22"/>
@@ -7801,7 +7801,7 @@
       </c>
       <c r="C7" s="21">
         <f>SUM(C5:C6)</f>
-        <v>0</v>
+        <v>1744.23</v>
       </c>
       <c r="D7" s="21">
         <f>SUM(D5:D6)</f>
@@ -7809,7 +7809,7 @@
       </c>
       <c r="E7" s="21">
         <f>SUM(E5:E6)</f>
-        <v>1379.75</v>
+        <v>3123.98</v>
       </c>
       <c r="F7" s="22"/>
       <c r="G7" s="22"/>
@@ -8059,7 +8059,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -8092,14 +8092,14 @@
         <v>0</v>
       </c>
       <c r="C2" s="18">
-        <v>0</v>
+        <v>5.3</v>
       </c>
       <c r="D2" s="18">
         <v>0</v>
       </c>
       <c r="E2" s="20">
         <f>SUM(B2:D2)</f>
-        <v>0</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -8112,7 +8112,7 @@
       </c>
       <c r="C3" s="19">
         <f>SUM(C2:C2)</f>
-        <v>0</v>
+        <v>5.3</v>
       </c>
       <c r="D3" s="19">
         <f>SUM(D2:D2)</f>
@@ -8120,7 +8120,7 @@
       </c>
       <c r="E3" s="19">
         <f>SUM(E2:E2)</f>
-        <v>0</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -8131,14 +8131,14 @@
         <v>0</v>
       </c>
       <c r="C4" s="18">
-        <v>0</v>
+        <v>1932.17</v>
       </c>
       <c r="D4" s="18">
         <v>0</v>
       </c>
       <c r="E4" s="20">
         <f>SUM(B4:D4)</f>
-        <v>0</v>
+        <v>1932.17</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -8151,7 +8151,7 @@
       </c>
       <c r="C5" s="21">
         <f>SUM(C4:C4)</f>
-        <v>0</v>
+        <v>1932.17</v>
       </c>
       <c r="D5" s="21">
         <f>SUM(D4:D4)</f>
@@ -8159,7 +8159,7 @@
       </c>
       <c r="E5" s="21">
         <f>SUM(E4:E4)</f>
-        <v>0</v>
+        <v>1932.17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>